<commit_message>
add method for correct reading .xlsx cells values from formulas
</commit_message>
<xml_diff>
--- a/HashMap/workbook.xlsx
+++ b/HashMap/workbook.xlsx
@@ -63,7 +63,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="2">
@@ -73,7 +73,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="4">
@@ -88,82 +88,82 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="22">
@@ -173,112 +173,112 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>9.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="45">
@@ -288,167 +288,167 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="79">
@@ -458,12 +458,12 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="82">
@@ -473,92 +473,92 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="101">
@@ -569,10 +569,10 @@
         <v>1.0</v>
       </c>
       <c r="C101">
-        <f>IF(A101&gt;=10,TRUE())</f>
+        <f>IF(A101&gt;=10,TRUE())*1</f>
       </c>
       <c r="D101">
-        <f>IF(C101=1,B101)</f>
+        <f>IF(C101=1,B101)*1</f>
       </c>
     </row>
     <row r="102">
@@ -583,10 +583,10 @@
         <v>2.0</v>
       </c>
       <c r="C102">
-        <f>IF(A102&gt;=10,TRUE())</f>
+        <f>IF(A102&gt;=10,TRUE())*1</f>
       </c>
       <c r="D102">
-        <f>IF(C102=1,B102)</f>
+        <f>IF(C102=1,B102)*1</f>
       </c>
     </row>
     <row r="103">
@@ -597,10 +597,10 @@
         <v>3.0</v>
       </c>
       <c r="C103">
-        <f>IF(A103&gt;=10,TRUE())</f>
+        <f>IF(A103&gt;=10,TRUE())*1</f>
       </c>
       <c r="D103">
-        <f>IF(C103=1,B103)</f>
+        <f>IF(C103=1,B103)*1</f>
       </c>
     </row>
     <row r="104">
@@ -611,10 +611,10 @@
         <v>4.0</v>
       </c>
       <c r="C104">
-        <f>IF(A104&gt;=10,TRUE())</f>
+        <f>IF(A104&gt;=10,TRUE())*1</f>
       </c>
       <c r="D104">
-        <f>IF(C104=1,B104)</f>
+        <f>IF(C104=1,B104)*1</f>
       </c>
     </row>
     <row r="105">
@@ -625,10 +625,10 @@
         <v>5.0</v>
       </c>
       <c r="C105">
-        <f>IF(A105&gt;=10,TRUE())</f>
+        <f>IF(A105&gt;=10,TRUE())*1</f>
       </c>
       <c r="D105">
-        <f>IF(C105=1,B105)</f>
+        <f>IF(C105=1,B105)*1</f>
       </c>
     </row>
     <row r="106">
@@ -639,10 +639,10 @@
         <v>6.0</v>
       </c>
       <c r="C106">
-        <f>IF(A106&gt;=10,TRUE())</f>
+        <f>IF(A106&gt;=10,TRUE())*1</f>
       </c>
       <c r="D106">
-        <f>IF(C106=1,B106)</f>
+        <f>IF(C106=1,B106)*1</f>
       </c>
     </row>
     <row r="107">
@@ -653,10 +653,10 @@
         <v>7.0</v>
       </c>
       <c r="C107">
-        <f>IF(A107&gt;=10,TRUE())</f>
+        <f>IF(A107&gt;=10,TRUE())*1</f>
       </c>
       <c r="D107">
-        <f>IF(C107=1,B107)</f>
+        <f>IF(C107=1,B107)*1</f>
       </c>
     </row>
     <row r="108">
@@ -667,10 +667,10 @@
         <v>8.0</v>
       </c>
       <c r="C108">
-        <f>IF(A108&gt;=10,TRUE())</f>
+        <f>IF(A108&gt;=10,TRUE())*1</f>
       </c>
       <c r="D108">
-        <f>IF(C108=1,B108)</f>
+        <f>IF(C108=1,B108)*1</f>
       </c>
     </row>
     <row r="109">
@@ -681,10 +681,10 @@
         <v>9.0</v>
       </c>
       <c r="C109">
-        <f>IF(A109&gt;=10,TRUE())</f>
+        <f>IF(A109&gt;=10,TRUE())*1</f>
       </c>
       <c r="D109">
-        <f>IF(C109=1,B109)</f>
+        <f>IF(C109=1,B109)*1</f>
       </c>
     </row>
     <row r="110">
@@ -695,10 +695,10 @@
         <v>10.0</v>
       </c>
       <c r="C110">
-        <f>IF(A110&gt;=10,TRUE())</f>
+        <f>IF(A110&gt;=10,TRUE())*1</f>
       </c>
       <c r="D110">
-        <f>IF(C110=1,B110)</f>
+        <f>IF(C110=1,B110)*1</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test for hashN method
</commit_message>
<xml_diff>
--- a/HashMap/workbook.xlsx
+++ b/HashMap/workbook.xlsx
@@ -63,72 +63,72 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="15">
@@ -138,27 +138,27 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="21">
@@ -168,42 +168,42 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="30">
@@ -223,32 +223,32 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>10.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="39">
@@ -258,202 +258,202 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>4.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>8.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>10.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>5.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>7.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>9.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>8.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="80">
@@ -463,102 +463,102 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="101">

</xml_diff>